<commit_message>
Add status and create_at field in GradeTable , Update frontend to use data from backend to show
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScorP1on\Desktop\grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98671A2-35AB-4704-A85E-8551AC558595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ABDA88-A741-4ACC-92B4-DCC0B6ED7BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>std_id</t>
   </si>
@@ -42,15 +42,6 @@
     <t>midterm</t>
   </si>
   <si>
-    <t>final</t>
-  </si>
-  <si>
-    <t>as1</t>
-  </si>
-  <si>
-    <t>as2</t>
-  </si>
-  <si>
     <t>pattana sapp</t>
   </si>
   <si>
@@ -63,7 +54,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>cn102</t>
+    <t>cn101</t>
   </si>
 </sst>
 </file>
@@ -405,7 +396,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F1" sqref="F1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,40 +420,25 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>6210612831</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>25</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -470,25 +446,16 @@
         <v>6301610595</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>50</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-      <c r="H3">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update frontend load data from backend
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\endless_project\grade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScorP1on\Desktop\grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E143B5-415E-4B5A-AD6D-FDEE84EF5846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723052A2-3711-489F-9E6C-8B998558A32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>std_id</t>
   </si>
@@ -36,9 +36,6 @@
     <t>subject</t>
   </si>
   <si>
-    <t>grade</t>
-  </si>
-  <si>
     <t>midterm</t>
   </si>
   <si>
@@ -48,19 +45,13 @@
     <t>tipkridta boonma</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>cn101</t>
-  </si>
-  <si>
     <t>nattanan</t>
   </si>
   <si>
     <t>nattanan naw</t>
+  </si>
+  <si>
+    <t>cn103</t>
   </si>
 </sst>
 </file>
@@ -71,7 +62,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -402,12 +393,12 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="18.25" customWidth="1"/>
+    <col min="1" max="11" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -422,9 +413,6 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -435,15 +423,12 @@
         <v>6210612831</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>25</v>
       </c>
     </row>
@@ -452,62 +437,53 @@
         <v>6301610595</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="D3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6210612567</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6210612566</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update create table backend,send grade table info to frontend
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScorP1on\Desktop\grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955F6C03-EA4F-4B45-A835-F5ABED0BE750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE297173-F554-4BA8-8581-006D457D098F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>subject</t>
-  </si>
-  <si>
     <t>midterm</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>subject d</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,16 +427,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -446,10 +446,10 @@
         <v>6210612831</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -466,10 +466,10 @@
         <v>6301610595</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -486,10 +486,10 @@
         <v>6210612567</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -506,10 +506,10 @@
         <v>6210612566</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>